<commit_message>
Atualizado por script em 22-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/bosnia-and-herzegovina_premijer-liga-bih_2023-2024.xlsx
+++ b/2023/bosnia-and-herzegovina_premijer-liga-bih_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V82"/>
+  <dimension ref="A1:V83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8001,6 +8001,98 @@
         </is>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>bosnia-and-herzegovina</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>premijer-liga-bih</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E83" s="2" t="n">
+        <v>45252.75</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Zrinjski</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>3</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Siroki Brijeg</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>03/09/2023 08:12</t>
+        </is>
+      </c>
+      <c r="L83" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>22/11/2023 17:59</t>
+        </is>
+      </c>
+      <c r="N83" t="n">
+        <v>4.72</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>03/09/2023 08:12</t>
+        </is>
+      </c>
+      <c r="P83" t="n">
+        <v>6.82</v>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>22/11/2023 17:59</t>
+        </is>
+      </c>
+      <c r="R83" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>03/09/2023 08:12</t>
+        </is>
+      </c>
+      <c r="T83" t="n">
+        <v>15.52</v>
+      </c>
+      <c r="U83" t="inlineStr">
+        <is>
+          <t>22/11/2023 17:59</t>
+        </is>
+      </c>
+      <c r="V83" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/bosnia-and-herzegovina/premijer-liga-bih/zrinjski-siroki-brijeg/l6bIl11G/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>